<commit_message>
offerte updatet en kleine wijziginen
</commit_message>
<xml_diff>
--- a/Documentatie/KT1/ad.3_Offerte.xlsx
+++ b/Documentatie/KT1/ad.3_Offerte.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Patrick\Downloads\Medex\Documentatie\KT1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Patrick\Documents\GitHub\WeekPlanner\Documentatie\KT1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -237,7 +237,7 @@
     <tableColumn id="12" name="Korting" dataDxfId="4"/>
     <tableColumn id="11" name="Bedrag" dataDxfId="3" dataCellStyle="Currency"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -247,7 +247,7 @@
   <tableColumns count="1">
     <tableColumn id="1" name="Column1" dataDxfId="0" dataCellStyle="Currency"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -517,7 +517,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>